<commit_message>
Changed to Java enterprise edition 1.8
</commit_message>
<xml_diff>
--- a/src/test/java/com/oracle/ICICI/HCM/databank/ICICIDataBank.xlsx
+++ b/src/test/java/com/oracle/ICICI/HCM/databank/ICICIDataBank.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA6445F3-E275-475D-9F5E-1D151935BA47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14100" windowHeight="6080" firstSheet="10" activeTab="10"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="10" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReviewPeriod" sheetId="1" r:id="rId1"/>
@@ -401,7 +402,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="165" formatCode="mm\-dd\-yyyy\ h:mm\ AM/PM"/>
@@ -581,6 +582,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -616,6 +634,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -791,21 +826,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="8.7265625" style="1"/>
-    <col min="5" max="5" width="14.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <col min="2" max="2" width="38.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.7109375" style="1"/>
+    <col min="5" max="5" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.7109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -822,7 +857,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -845,20 +880,20 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>19</v>
       </c>
@@ -866,7 +901,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -881,23 +916,23 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.54296875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -917,7 +952,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>313506</v>
       </c>
@@ -944,23 +979,23 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="12.90625" customWidth="1"/>
-    <col min="2" max="2" width="13.7265625" customWidth="1"/>
-    <col min="3" max="3" width="19.26953125" customWidth="1"/>
-    <col min="4" max="4" width="18.81640625" customWidth="1"/>
-    <col min="5" max="5" width="17.54296875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -980,7 +1015,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>600584</v>
       </c>
@@ -1002,29 +1037,29 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="16.08984375" customWidth="1"/>
-    <col min="3" max="3" width="18.6328125" customWidth="1"/>
-    <col min="4" max="4" width="12.36328125" customWidth="1"/>
-    <col min="5" max="5" width="15.36328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -1044,7 +1079,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>100004</v>
       </c>
@@ -1070,23 +1105,23 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="13.36328125" customWidth="1"/>
-    <col min="3" max="3" width="20.54296875" customWidth="1"/>
-    <col min="4" max="4" width="17.1796875" customWidth="1"/>
-    <col min="5" max="5" width="16.90625" customWidth="1"/>
-    <col min="6" max="6" width="16.54296875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -1103,7 +1138,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>600434</v>
       </c>
@@ -1122,27 +1157,27 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="3" max="3" width="20.08984375" customWidth="1"/>
-    <col min="5" max="5" width="22.453125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -1162,7 +1197,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>313506</v>
       </c>
@@ -1188,19 +1223,19 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="15.26953125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -1220,7 +1255,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>313506</v>
       </c>
@@ -1246,22 +1281,22 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="17.54296875" customWidth="1"/>
-    <col min="3" max="3" width="15.26953125" customWidth="1"/>
-    <col min="4" max="4" width="13.54296875" customWidth="1"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -1278,7 +1313,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>100042</v>
       </c>
@@ -1295,7 +1330,7 @@
         <v>44358</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>100042</v>
       </c>
@@ -1312,22 +1347,22 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="20.54296875" customWidth="1"/>
-    <col min="3" max="3" width="12.08984375" customWidth="1"/>
-    <col min="4" max="4" width="13.26953125" customWidth="1"/>
-    <col min="5" max="5" width="14.1796875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -1347,7 +1382,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>401574</v>
       </c>
@@ -1369,31 +1404,31 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-1100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="11.1796875" customWidth="1"/>
-    <col min="3" max="3" width="15.36328125" customWidth="1"/>
-    <col min="4" max="4" width="17.453125" customWidth="1"/>
-    <col min="5" max="5" width="20.08984375" customWidth="1"/>
-    <col min="6" max="6" width="14.7265625" customWidth="1"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
     <col min="7" max="7" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -1416,7 +1451,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="153.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="153.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>118037</v>
       </c>
@@ -1433,7 +1468,7 @@
         <v>44435.739583333336</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>118037</v>
       </c>
@@ -1462,23 +1497,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.7265625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1501,7 +1536,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1530,23 +1565,23 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="18.26953125" customWidth="1"/>
-    <col min="3" max="3" width="18.08984375" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" customWidth="1"/>
-    <col min="5" max="5" width="18.453125" customWidth="1"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -1566,7 +1601,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>313506</v>
       </c>
@@ -1588,33 +1623,33 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="Welcome@1"/>
+    <hyperlink ref="B2" r:id="rId1" display="Welcome@1" xr:uid="{00000000-0004-0000-1300-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="15.1796875" customWidth="1"/>
-    <col min="3" max="3" width="20.36328125" customWidth="1"/>
-    <col min="4" max="4" width="14.54296875" customWidth="1"/>
-    <col min="5" max="5" width="12.54296875" customWidth="1"/>
-    <col min="6" max="6" width="17.26953125" customWidth="1"/>
-    <col min="7" max="7" width="25.453125" customWidth="1"/>
-    <col min="8" max="8" width="18.26953125" customWidth="1"/>
-    <col min="9" max="9" width="18.36328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1"/>
+    <col min="7" max="7" width="25.42578125" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -1643,7 +1678,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>167563</v>
       </c>
@@ -1663,7 +1698,7 @@
         <v>44438</v>
       </c>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G17" t="s">
         <v>73</v>
       </c>
@@ -1675,27 +1710,27 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="16.1796875" customWidth="1"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="19.81640625" customWidth="1"/>
-    <col min="5" max="6" width="19.36328125" customWidth="1"/>
-    <col min="7" max="7" width="14.453125" customWidth="1"/>
-    <col min="8" max="9" width="18.90625" customWidth="1"/>
-    <col min="10" max="10" width="22.36328125" customWidth="1"/>
-    <col min="11" max="11" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.453125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <col min="4" max="4" width="19.85546875" customWidth="1"/>
+    <col min="5" max="6" width="19.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
+    <col min="8" max="9" width="18.85546875" customWidth="1"/>
+    <col min="10" max="10" width="22.42578125" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -1730,7 +1765,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>313506</v>
       </c>
@@ -1741,13 +1776,13 @@
         <v>71</v>
       </c>
       <c r="D2" s="15">
-        <v>44441</v>
+        <v>44520</v>
       </c>
       <c r="E2" s="15" t="s">
         <v>85</v>
       </c>
       <c r="F2" s="15">
-        <v>44441</v>
+        <v>44520</v>
       </c>
       <c r="G2" t="s">
         <v>72</v>
@@ -1756,7 +1791,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>162435</v>
       </c>
@@ -1770,16 +1805,16 @@
         <v>87</v>
       </c>
       <c r="J3" s="8">
-        <v>44441</v>
+        <v>44520</v>
       </c>
       <c r="K3" s="8">
-        <v>44441</v>
+        <v>44520</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="Welcome@1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B2" r:id="rId1" display="Welcome@1" xr:uid="{00000000-0004-0000-1500-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-1500-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -1787,25 +1822,25 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="10.81640625" customWidth="1"/>
-    <col min="3" max="3" width="27.7265625" customWidth="1"/>
-    <col min="4" max="4" width="25.81640625" customWidth="1"/>
-    <col min="5" max="5" width="21.7265625" customWidth="1"/>
-    <col min="6" max="6" width="16.7265625" customWidth="1"/>
-    <col min="7" max="7" width="17.54296875" customWidth="1"/>
-    <col min="8" max="8" width="29.7265625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" customWidth="1"/>
+    <col min="8" max="8" width="29.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -1834,7 +1869,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>101917</v>
       </c>
@@ -1865,7 +1900,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="Welcome@1"/>
+    <hyperlink ref="B2" r:id="rId1" display="Welcome@1" xr:uid="{00000000-0004-0000-1600-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -1873,26 +1908,26 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="14.7265625" customWidth="1"/>
-    <col min="3" max="3" width="15.7265625" customWidth="1"/>
-    <col min="4" max="4" width="17.1796875" customWidth="1"/>
-    <col min="5" max="5" width="14.08984375" customWidth="1"/>
-    <col min="6" max="6" width="22.36328125" customWidth="1"/>
-    <col min="7" max="7" width="22.26953125" customWidth="1"/>
-    <col min="8" max="8" width="18.36328125" customWidth="1"/>
-    <col min="9" max="9" width="22.6328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" customWidth="1"/>
+    <col min="9" max="9" width="22.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -1918,7 +1953,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>380965</v>
       </c>
@@ -1947,7 +1982,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="Welcome@1"/>
+    <hyperlink ref="B2" r:id="rId1" display="Welcome@1" xr:uid="{00000000-0004-0000-1700-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -1955,27 +1990,27 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="11.90625" customWidth="1"/>
-    <col min="3" max="3" width="17.453125" customWidth="1"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
     <col min="4" max="4" width="18" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.26953125" customWidth="1"/>
-    <col min="6" max="6" width="15.36328125" customWidth="1"/>
-    <col min="7" max="7" width="17.26953125" customWidth="1"/>
-    <col min="8" max="8" width="20.08984375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="17.81640625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="13.08984375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -2007,7 +2042,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>167563</v>
       </c>
@@ -2036,24 +2071,24 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="12.453125" customWidth="1"/>
-    <col min="3" max="3" width="12.6328125" customWidth="1"/>
-    <col min="4" max="4" width="14.36328125" customWidth="1"/>
-    <col min="5" max="5" width="16.90625" customWidth="1"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="44.7265625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <col min="7" max="7" width="44.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -2076,7 +2111,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>391986</v>
       </c>
@@ -2101,30 +2136,30 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-1900-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="11.26953125" customWidth="1"/>
-    <col min="3" max="3" width="16.26953125" customWidth="1"/>
-    <col min="4" max="5" width="15.81640625" customWidth="1"/>
-    <col min="6" max="7" width="18.54296875" customWidth="1"/>
-    <col min="8" max="8" width="20.1796875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="4" max="5" width="15.85546875" customWidth="1"/>
+    <col min="6" max="7" width="18.5703125" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -2150,7 +2185,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>313506</v>
       </c>
@@ -2178,30 +2213,30 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="Welcome@1"/>
+    <hyperlink ref="B2" r:id="rId1" display="Welcome@1" xr:uid="{00000000-0004-0000-1A00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="18.453125" customWidth="1"/>
-    <col min="3" max="3" width="14.90625" customWidth="1"/>
-    <col min="4" max="4" width="12.36328125" customWidth="1"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="13.6328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -2221,7 +2256,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>100004</v>
       </c>
@@ -2247,23 +2282,23 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="18.453125" customWidth="1"/>
-    <col min="3" max="3" width="20.453125" customWidth="1"/>
-    <col min="4" max="4" width="17.54296875" customWidth="1"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="19.08984375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -2274,7 +2309,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>170058</v>
       </c>
@@ -2293,26 +2328,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="25.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1796875" bestFit="1" customWidth="1"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.54296875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2338,7 +2373,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -2364,7 +2399,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -2396,23 +2431,23 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="19.1796875" customWidth="1"/>
-    <col min="4" max="4" width="20.36328125" customWidth="1"/>
-    <col min="5" max="5" width="25.6328125" customWidth="1"/>
-    <col min="6" max="6" width="18.90625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -2432,7 +2467,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>300202</v>
       </c>
@@ -2452,7 +2487,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>300054</v>
       </c>
@@ -2478,22 +2513,22 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="14.36328125" customWidth="1"/>
-    <col min="4" max="4" width="12.1796875" customWidth="1"/>
-    <col min="5" max="5" width="15.81640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -2513,7 +2548,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>313506</v>
       </c>
@@ -2539,23 +2574,23 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="16.54296875" customWidth="1"/>
-    <col min="3" max="3" width="18.90625" customWidth="1"/>
-    <col min="4" max="4" width="19.7265625" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" customWidth="1"/>
-    <col min="6" max="6" width="17.26953125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -2575,7 +2610,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>313506</v>
       </c>
@@ -2601,24 +2636,24 @@
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="14.6328125" customWidth="1"/>
-    <col min="3" max="3" width="15.90625" customWidth="1"/>
-    <col min="4" max="4" width="16.08984375" customWidth="1"/>
-    <col min="5" max="5" width="20.36328125" customWidth="1"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" customWidth="1"/>
     <col min="6" max="6" width="31" customWidth="1"/>
-    <col min="7" max="7" width="41.453125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <col min="7" max="7" width="41.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -2641,7 +2676,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="10" customFormat="1" ht="53.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" s="10" customFormat="1" ht="53.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <v>410443</v>
       </c>
@@ -2666,33 +2701,33 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="Welcome@1"/>
+    <hyperlink ref="B2" r:id="rId1" display="Welcome@1" xr:uid="{00000000-0004-0000-2000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="39.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.26953125" style="1" customWidth="1"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="26" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="12" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.7265625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <col min="6" max="6" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.7109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
@@ -2718,7 +2753,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>36</v>
       </c>
@@ -2750,22 +2785,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="17.26953125" customWidth="1"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="17.28515625" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.54296875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2782,7 +2817,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>48</v>
       </c>
@@ -2805,22 +2840,22 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="25" customWidth="1"/>
-    <col min="7" max="7" width="19.7265625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <col min="7" max="7" width="19.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>19</v>
       </c>
@@ -2846,7 +2881,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -2879,16 +2914,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2902,7 +2937,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -2922,19 +2957,19 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="4" max="4" width="22.453125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2948,7 +2983,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>46</v>
       </c>
@@ -2968,22 +3003,22 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="28.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="28.1796875" customWidth="1"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="28.140625" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.54296875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3000,7 +3035,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>45</v>
       </c>

</xml_diff>